<commit_message>
Updated genenames for galactose
</commit_message>
<xml_diff>
--- a/Models/model.xlsx
+++ b/Models/model.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="860">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="862">
   <si>
     <t>#</t>
   </si>
@@ -2603,6 +2603,12 @@
   </si>
   <si>
     <t>0.804 1,3bis-phosphoglycerate[c] + 18.4 acetyl-CoA[c] + 0.197 alpha-D-glucose 6-phosphate[c] + 19.6 ATP[c] + 0.918 glycerone phosphate[c] + 0.316 nad+[c] + 29.9 NADPH[c] + 0.00208 NADPH[m] + 0.572 O2[c] + 0.00416 pyruvate[m] + 0.00208 oxaloacetate[c] =&gt; 19.6 ADP[c] + 1.4 CO2[c] + 18.4 coenzyme A[c] + 0.316 NADH[c] + 29.9 nadp+[c] + 0.00208 nadp+[m] + 21.6 phosphate[c] + growthLipid[c]</t>
+  </si>
+  <si>
+    <t>YBR019C</t>
+  </si>
+  <si>
+    <t>YBR018C</t>
   </si>
 </sst>
 </file>
@@ -2969,8 +2975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3376,7 +3382,7 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>860</v>
       </c>
       <c r="J16" t="s">
         <v>60</v>
@@ -3399,7 +3405,7 @@
         <v>70</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>861</v>
       </c>
       <c r="J17" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
chore: added output model files
</commit_message>
<xml_diff>
--- a/Models/model.xlsx
+++ b/Models/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivand/Documents/GitHub/ECM_Yeast/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B60F3F43-161D-8A4D-89CA-69B8318EC963}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92042D01-DE6A-3147-AE90-7EC7345DFCBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18620" windowHeight="23440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="20160" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RXNS" sheetId="1" r:id="rId1"/>
@@ -2735,9 +2735,6 @@
     <t>NADH[c] + ubiquinone-6[m] =&gt; nad+[c] + ubiquinol-6[m]</t>
   </si>
   <si>
-    <t>ubiquinol-6[m] + 2 ferricytochrome c[m] + 1.5 h+[m] =&gt; ubiquinone-6[m] + 2 ferrocytochrome c[m] + 1.5 h+[i]</t>
-  </si>
-  <si>
     <t>0.25 O2[c] + ferrocytochrome c[m] + 2 h+[m] =&gt; ferricytochrome c[m] + 0.5 H2O[m] + h+[i]</t>
   </si>
   <si>
@@ -2892,6 +2889,9 @@
   </si>
   <si>
     <t>acetate[c] + ATP[c] + H2O[c] + coenzyme A[c] =&gt; acetyl-CoA[c] + AMP[c] + 2 phosphate[c]</t>
+  </si>
+  <si>
+    <t>ubiquinol-6[m] + 2 ferricytochrome c[m] + 2 h+[m] =&gt; ubiquinone-6[m] + 2 ferrocytochrome c[m] + 2 h+[i]</t>
   </si>
 </sst>
 </file>
@@ -3259,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="C41" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3598,7 +3598,7 @@
         <v>669</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>55</v>
@@ -3624,7 +3624,7 @@
         <v>59</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>664</v>
@@ -3647,7 +3647,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>665</v>
@@ -3673,7 +3673,7 @@
         <v>64</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>666</v>
@@ -3699,7 +3699,7 @@
         <v>66</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>713</v>
@@ -3725,7 +3725,7 @@
         <v>708</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>70</v>
@@ -3751,7 +3751,7 @@
         <v>709</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>714</v>
@@ -3777,7 +3777,7 @@
         <v>880</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>74</v>
@@ -3803,7 +3803,7 @@
         <v>808</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>77</v>
@@ -3826,7 +3826,7 @@
         <v>809</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>79</v>
@@ -3849,7 +3849,7 @@
         <v>800</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>715</v>
@@ -3872,7 +3872,7 @@
         <v>801</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>83</v>
@@ -3898,7 +3898,7 @@
         <v>797</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>558</v>
@@ -3924,7 +3924,7 @@
         <v>881</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>716</v>
@@ -3950,7 +3950,7 @@
         <v>90</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>717</v>
@@ -3976,7 +3976,7 @@
         <v>92</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>93</v>
@@ -4002,7 +4002,7 @@
         <v>882</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>718</v>
@@ -4028,7 +4028,7 @@
         <v>98</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>99</v>
@@ -4054,7 +4054,7 @@
         <v>101</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>102</v>
@@ -4077,7 +4077,7 @@
         <v>104</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>105</v>
@@ -4103,7 +4103,7 @@
         <v>107</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>108</v>
@@ -4126,7 +4126,7 @@
         <v>710</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>111</v>
@@ -4149,7 +4149,7 @@
         <v>711</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>108</v>
@@ -4172,7 +4172,7 @@
         <v>810</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>114</v>
@@ -4198,7 +4198,7 @@
         <v>883</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>117</v>
@@ -4224,7 +4224,7 @@
         <v>120</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>719</v>
@@ -4250,7 +4250,7 @@
         <v>122</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>720</v>
@@ -4276,7 +4276,7 @@
         <v>884</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>124</v>
@@ -4302,7 +4302,7 @@
         <v>885</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>721</v>
@@ -4328,7 +4328,7 @@
         <v>129</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>576</v>
@@ -4354,7 +4354,7 @@
         <v>886</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>133</v>
@@ -4397,7 +4397,7 @@
         <v>139</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>722</v>
@@ -4420,10 +4420,10 @@
         <v>692</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>141</v>
@@ -4449,7 +4449,7 @@
         <v>661</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>723</v>
@@ -4478,7 +4478,7 @@
         <v>144</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>145</v>
@@ -4504,7 +4504,7 @@
         <v>887</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>724</v>
@@ -4530,7 +4530,7 @@
         <v>894</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>149</v>
@@ -4553,7 +4553,7 @@
         <v>152</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>153</v>
@@ -4579,7 +4579,7 @@
         <v>155</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>538</v>
@@ -4605,7 +4605,7 @@
         <v>157</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>538</v>
@@ -4628,7 +4628,7 @@
         <v>662</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>554</v>
@@ -4651,7 +4651,7 @@
         <v>650</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>725</v>
@@ -4668,19 +4668,19 @@
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
-        <v>791</v>
+        <v>158</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>792</v>
+        <v>697</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>948</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>727</v>
+        <v>159</v>
       </c>
       <c r="J60" s="6" t="s">
         <v>130</v>
@@ -4688,22 +4688,25 @@
       <c r="L60" s="6" t="s">
         <v>147</v>
       </c>
+      <c r="N60" s="6" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>697</v>
+        <v>161</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>897</v>
+        <v>162</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>949</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="J61" s="6" t="s">
         <v>130</v>
@@ -4712,33 +4715,30 @@
         <v>147</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
-        <v>160</v>
+        <v>791</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>161</v>
+        <v>792</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>162</v>
+        <v>900</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>163</v>
+        <v>727</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>130</v>
       </c>
       <c r="L62" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="N62" s="6" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.2">
@@ -4752,7 +4752,7 @@
         <v>901</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>583</v>
@@ -4775,7 +4775,7 @@
         <v>902</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>726</v>
@@ -4795,10 +4795,10 @@
         <v>700</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>903</v>
+        <v>955</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>728</v>
@@ -4818,10 +4818,10 @@
         <v>701</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>729</v>
@@ -4844,10 +4844,10 @@
         <v>702</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>730</v>

</xml_diff>